<commit_message>
fix issues with importing email and phone numbers for a contact
</commit_message>
<xml_diff>
--- a/demodata/partners/samplePartnerImport.xlsx
+++ b/demodata/partners/samplePartnerImport.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t xml:space="preserve">FirstName</t>
   </si>
@@ -28,6 +28,9 @@
     <t xml:space="preserve">FamilyName</t>
   </si>
   <si>
+    <t xml:space="preserve">Title</t>
+  </si>
+  <si>
     <t xml:space="preserve">Gender</t>
   </si>
   <si>
@@ -46,12 +49,21 @@
     <t xml:space="preserve">Email</t>
   </si>
   <si>
+    <t xml:space="preserve">Mobile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phone</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dalton</t>
   </si>
   <si>
     <t xml:space="preserve">Lloyd</t>
   </si>
   <si>
+    <t xml:space="preserve">Mr</t>
+  </si>
+  <si>
     <t xml:space="preserve">Male</t>
   </si>
   <si>
@@ -70,6 +82,12 @@
     <t xml:space="preserve">dignissim.pharetra@sapienCrasdolor.org</t>
   </si>
   <si>
+    <t xml:space="preserve">+49 151 123456</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+49 1234 123456</t>
+  </si>
+  <si>
     <t xml:space="preserve">Julian</t>
   </si>
   <si>
@@ -86,6 +104,9 @@
   </si>
   <si>
     <t xml:space="preserve">mauris.blandit.mattis@ac.ca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+49 151 123457</t>
   </si>
 </sst>
 </file>
@@ -100,6 +121,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -181,22 +203,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="34.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="4.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="34.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.46"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -224,57 +249,81 @@
       <c r="H1" s="0" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>21</v>
+      <c r="I3" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
partner import: fixes for import of consent ignore empty rows. update example files
</commit_message>
<xml_diff>
--- a/demodata/partners/samplePartnerImport.xlsx
+++ b/demodata/partners/samplePartnerImport.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
   <si>
     <t xml:space="preserve">FirstName</t>
   </si>
@@ -55,6 +55,36 @@
     <t xml:space="preserve">Phone</t>
   </si>
   <si>
+    <t xml:space="preserve">Category1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ConsentChannel1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ConsentWhen1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ConsentType1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ConsentPurpose1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ConsentChannel2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ConsentWhen2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ConsentType2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ConsentPurpose2</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dalton</t>
   </si>
   <si>
@@ -88,6 +118,30 @@
     <t xml:space="preserve">+49 1234 123456</t>
   </si>
   <si>
+    <t xml:space="preserve">VOLUNTEER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX-WORKER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONVERSATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMAIL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEWSLETTER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LETTER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADDRESS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GR</t>
+  </si>
+  <si>
     <t xml:space="preserve">Julian</t>
   </si>
   <si>
@@ -107,16 +161,20 @@
   </si>
   <si>
     <t xml:space="preserve">+49 151 123457</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STAFF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -137,6 +195,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -181,8 +244,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -203,10 +278,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -222,109 +297,192 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="34.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="12.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="15.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="15.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="13.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="13.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="15.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="15.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="13.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="13.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="15.88"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" s="0" t="s">
+    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>21</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O2" s="3" t="n">
+        <v>44213</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S2" s="3" t="n">
+        <v>44214</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="0" t="s">
+      <c r="A3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="J3" s="0" t="s">
+      <c r="E3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="I3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
delete contact: delete banking details usage add IBAN column to sample contact import files.
</commit_message>
<xml_diff>
--- a/demodata/partners/samplePartnerImport.xlsx
+++ b/demodata/partners/samplePartnerImport.xlsx
@@ -13,14 +13,14 @@
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="50">
   <si>
     <t xml:space="preserve">FirstName</t>
   </si>
@@ -85,6 +85,9 @@
     <t xml:space="preserve">ConsentPurpose2</t>
   </si>
   <si>
+    <t xml:space="preserve">IBAN1</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dalton</t>
   </si>
   <si>
@@ -140,6 +143,9 @@
   </si>
   <si>
     <t xml:space="preserve">GR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE02700202700010108669</t>
   </si>
   <si>
     <t xml:space="preserve">Julian</t>
@@ -179,7 +185,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -200,6 +205,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -244,21 +250,25 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -278,35 +288,37 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:V3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="4.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="34.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="12.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="15.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="15.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="13.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="13.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="15.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="15.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="13.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="13.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="15.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="4.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="20.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="9.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="15.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="7.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="34.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="14.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="15.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="12.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="12.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="15.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="13.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="13.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="15.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="15.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="13.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="13.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="15.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="24.17"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="23" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -373,124 +385,120 @@
       <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="O2" s="3" t="n">
         <v>44213</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="S2" s="3" t="n">
         <v>44214</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="V2" s="4" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="K3" s="1"/>
+        <v>48</v>
+      </c>
       <c r="L3" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
+        <v>49</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CSeite &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
more work on contact import. add examples and tests for importing organisations. add column OrganisationName. only require at least one of address, email, phone or IBAN for a valid contact. allow partial address, but set sendmail to false.
</commit_message>
<xml_diff>
--- a/demodata/partners/samplePartnerImport.xlsx
+++ b/demodata/partners/samplePartnerImport.xlsx
@@ -13,14 +13,17 @@
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="58">
+  <si>
+    <t xml:space="preserve">OrganisationName</t>
+  </si>
   <si>
     <t xml:space="preserve">FirstName</t>
   </si>
@@ -130,6 +133,9 @@
     <t xml:space="preserve">CONVERSATION</t>
   </si>
   <si>
+    <t xml:space="preserve">17.01.21</t>
+  </si>
+  <si>
     <t xml:space="preserve">EMAIL</t>
   </si>
   <si>
@@ -139,6 +145,9 @@
     <t xml:space="preserve">LETTER</t>
   </si>
   <si>
+    <t xml:space="preserve">18.01.21</t>
+  </si>
+  <si>
     <t xml:space="preserve">ADDRESS</t>
   </si>
   <si>
@@ -170,6 +179,21 @@
   </si>
   <si>
     <t xml:space="preserve">STAFF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Smith</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AT021860000012387890</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tree Foundation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info@example.org</t>
   </si>
 </sst>
 </file>
@@ -178,9 +202,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -200,12 +224,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -250,25 +268,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -288,217 +294,250 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V3"/>
+  <dimension ref="A1:W5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="4.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="20.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="9.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="15.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="7.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="34.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="14.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="15.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="12.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="12.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="15.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="13.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="13.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="15.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="15.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="13.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="13.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="15.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="24.17"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="23" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="4.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="7.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="34.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="14.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="9.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="15.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="13.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="13.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="15.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="15.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="13.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="13.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="15.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="23.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="0" t="s">
         <v>21</v>
+      </c>
+      <c r="W1" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N2" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="O2" s="3" t="n">
-        <v>44213</v>
+      <c r="O2" s="0" t="s">
+        <v>36</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="Q2" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="S2" s="3" t="n">
-        <v>44214</v>
+      <c r="R2" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="S2" s="0" t="s">
+        <v>40</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="V2" s="4" t="s">
         <v>41</v>
+      </c>
+      <c r="U2" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="V2" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="W2" s="0" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="B3" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I3" s="1" t="s">
+      <c r="E3" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="G3" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="H3" s="0" t="s">
         <v>49</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="M3" s="0" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="W4" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;A</oddHeader>
-    <oddFooter>&amp;CSeite &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>